<commit_message>
inconsistencia nos dados do banco
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/recomendacao_compra_final.xlsx
+++ b/dados/ADD/Dados_ADD_PF/recomendacao_compra_final.xlsx
@@ -38753,7 +38753,7 @@
         <v>46</v>
       </c>
       <c r="W379">
-        <v>803.8</v>
+        <v>803.8000000000001</v>
       </c>
       <c r="X379">
         <v>2</v>
@@ -44344,7 +44344,7 @@
         <v>98</v>
       </c>
       <c r="W437">
-        <v>553.1899999999999</v>
+        <v>553.1900000000001</v>
       </c>
       <c r="X437">
         <v>35</v>
@@ -47643,7 +47643,7 @@
         <v>700</v>
       </c>
       <c r="W471">
-        <v>7226.599999999999</v>
+        <v>7226.6</v>
       </c>
       <c r="X471">
         <v>57</v>
@@ -52464,7 +52464,7 @@
         <v>91</v>
       </c>
       <c r="W522">
-        <v>844.05</v>
+        <v>844.0500000000001</v>
       </c>
       <c r="X522">
         <v>12</v>
@@ -56995,7 +56995,7 @@
         <v>64</v>
       </c>
       <c r="W569">
-        <v>933.95</v>
+        <v>933.9499999999999</v>
       </c>
       <c r="X569">
         <v>4</v>

</xml_diff>